<commit_message>
plotted snow and snowmelt doc
</commit_message>
<xml_diff>
--- a/data/newrnet-chemistry/RI23_endmember_STDEV.xlsx
+++ b/data/newrnet-chemistry/RI23_endmember_STDEV.xlsx
@@ -9,6 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="SI Table" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="111">
   <si>
     <t xml:space="preserve">Sample ID</t>
   </si>
@@ -314,6 +315,45 @@
   </si>
   <si>
     <t xml:space="preserve">RI23-1061</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Table 2. Mean concentration values of potential hydrologic ﬂowpath tracers in each end-member. Units for Cl_x0001_..</t>
+  </si>
+  <si>
+    <t xml:space="preserve">End-member</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cl-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cl- STDV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Na+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ca2+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mg2+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H4SiO4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Snowmelt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Soil water wet site</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Soil water dry site</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Groundwater/baseflow</t>
   </si>
 </sst>
 </file>
@@ -418,10 +458,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AK20"/>
+  <dimension ref="A1:AK34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="5:5"/>
+      <selection pane="topLeft" activeCell="I24" activeCellId="0" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1918,6 +1958,101 @@
         <v>2.83</v>
       </c>
     </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="F25" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="G25" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="H25" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="I25" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="J25" s="0" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <f aca="false">AVERAGE(U18:U20)</f>
+        <v>4.289802042</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <f aca="false">STDEV(U18:U20)</f>
+        <v>2.95613349725257</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1927,4 +2062,27 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
ran all events with pca function looking good need refining em selection baseflow
</commit_message>
<xml_diff>
--- a/data/newrnet-chemistry/RI23_endmember_STDEV.xlsx
+++ b/data/newrnet-chemistry/RI23_endmember_STDEV.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="All data" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="SI Table" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Just tracers" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="217">
   <si>
     <t xml:space="preserve">Sample ID</t>
   </si>
@@ -354,6 +355,324 @@
   </si>
   <si>
     <t xml:space="preserve">Groundwater/baseflow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Si (mg/L)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mg (mg/L)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Na (mg/L)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ca (mg/L)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cl (mg/L)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOC (mg/L)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Soil water – Dry transect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.505 ± 0.089</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.335 ± 0.061</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.12 ± 0.10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.568 ± 0.028</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.90 ± 0.02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-91.29 ± 1.89</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-13.28 ± 0.05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.86 ± 1.04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Soil water - Wet transect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.279 ± NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.328 ± NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.858 ± NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.446 ± NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.736 ± NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-78.10 ± NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-11.58 ± NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.74 ± NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.114 ± 0.123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.137 ± 0.059</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.03 ± 0.17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.58 ± 0.14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.76 ± 0.22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-94.78 ± 8.57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-13.14 ± 1.24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.46 ± 1.03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.00 ± 0.95</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.75 ± 0.29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.21 ± 0.31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27.65 ± 1.37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.56 ± 0.09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-80.32 ± 1.15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-12.41 ± 0.53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.73 ± 0.51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.88 ± NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.753 ± NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.241 ± NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.51 ± NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.04 ± NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-77.61 ± 17.01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-11.18 ± 2.03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.39 ± 0.89</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.69 ± 2.83</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.11 ± 1.68</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.66 ± 1.26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12.6 ± 14.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.29 ± 2.19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-81.88 ± 7.61</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-12.64 ± 1.26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.13 ± 0.36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subwatershed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Endmember type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.505 ± 0.089 (3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.335 ± 0.061 (3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.12 ± 0.10 (3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.568 ± 0.028 (3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.90 ± 0.02 (3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-91.29 ± 1.89 (2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-13.28 ± 0.05 (2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.86 ± 1.04 (3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.279 ± NA (1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.328 ± NA (1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.858 ± NA (1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.446 ± NA (1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.736 ± NA (1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-78.10 ± NA (1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-11.58 ± NA (1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.74 ± NA (1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.114 ± 0.123 (3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.137 ± 0.059 (3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.03 ± 0.17 (3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.58 ± 0.14 (3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.76 ± 0.22 (3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-94.78 ± 8.57 (4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-13.14 ± 1.24 (4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.46 ± 1.03 (2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.00 ± 0.95 (2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.75 ± 0.29 (2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.21 ± 0.31 (2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27.65 ± 1.37 (2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.56 ± 0.09 (2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-80.32 ± 1.15 (2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-12.41 ± 0.53 (2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.73 ± 0.51 (2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.88 ± NA (1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.753 ± NA (1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.241 ± NA (1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.51 ± NA (1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.04 ± NA (1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-77.61 ± 17.01 (2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-11.18 ± 2.03 (2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.39 ± 0.89 (2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.69 ± 2.83 (3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.11 ± 1.68 (3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.66 ± 1.26 (3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12.60 ± 14.3 (3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.29 ± 2.19 (2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-81.88 ± 7.61 (2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-12.64 ± 1.26 (2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.13 ± 0.36 (2)</t>
   </si>
 </sst>
 </file>
@@ -364,11 +683,12 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -384,6 +704,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -428,7 +755,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -439,6 +766,14 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -460,11 +795,11 @@
   </sheetPr>
   <dimension ref="A1:AK34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I24" activeCellId="0" sqref="I24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="28.16"/>
   </cols>
@@ -2069,14 +2404,1488 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:J18"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.48"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+    </row>
+    <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:AMJ33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="27.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="28.16"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="ALL1" s="0"/>
+      <c r="ALM1" s="0"/>
+      <c r="ALN1" s="0"/>
+      <c r="ALO1" s="0"/>
+      <c r="ALP1" s="0"/>
+      <c r="ALQ1" s="0"/>
+      <c r="ALR1" s="0"/>
+      <c r="ALS1" s="0"/>
+      <c r="ALT1" s="0"/>
+      <c r="ALU1" s="0"/>
+      <c r="ALV1" s="0"/>
+      <c r="ALW1" s="0"/>
+      <c r="ALX1" s="0"/>
+      <c r="ALY1" s="0"/>
+      <c r="ALZ1" s="0"/>
+      <c r="AMA1" s="0"/>
+      <c r="AMB1" s="0"/>
+      <c r="AMC1" s="0"/>
+      <c r="AMD1" s="0"/>
+      <c r="AME1" s="0"/>
+      <c r="AMF1" s="0"/>
+      <c r="AMG1" s="0"/>
+      <c r="AMH1" s="0"/>
+      <c r="AMI1" s="0"/>
+      <c r="AMJ1" s="0"/>
+    </row>
+    <row r="2" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <v>0.429856652</v>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>0.396151045</v>
+      </c>
+      <c r="G2" s="1" t="n">
+        <v>-1.016981079</v>
+      </c>
+      <c r="H2" s="1" t="n">
+        <v>0.577446065</v>
+      </c>
+      <c r="I2" s="1" t="n">
+        <v>1.923457692</v>
+      </c>
+      <c r="J2" s="1" t="n">
+        <v>-93.641</v>
+      </c>
+      <c r="K2" s="1" t="n">
+        <v>-13.233</v>
+      </c>
+      <c r="L2" s="1" t="n">
+        <v>4.95</v>
+      </c>
+      <c r="ALL2" s="0"/>
+      <c r="ALM2" s="0"/>
+      <c r="ALN2" s="0"/>
+      <c r="ALO2" s="0"/>
+      <c r="ALP2" s="0"/>
+      <c r="ALQ2" s="0"/>
+      <c r="ALR2" s="0"/>
+      <c r="ALS2" s="0"/>
+      <c r="ALT2" s="0"/>
+      <c r="ALU2" s="0"/>
+      <c r="ALV2" s="0"/>
+      <c r="ALW2" s="0"/>
+      <c r="ALX2" s="0"/>
+      <c r="ALY2" s="0"/>
+      <c r="ALZ2" s="0"/>
+      <c r="AMA2" s="0"/>
+      <c r="AMB2" s="0"/>
+      <c r="AMC2" s="0"/>
+      <c r="AMD2" s="0"/>
+      <c r="AME2" s="0"/>
+      <c r="AMF2" s="0"/>
+      <c r="AMG2" s="0"/>
+      <c r="AMH2" s="0"/>
+      <c r="AMI2" s="0"/>
+      <c r="AMJ2" s="0"/>
+    </row>
+    <row r="3" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="1" t="n">
+        <v>0.60254712</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>0.334881921</v>
+      </c>
+      <c r="G3" s="1" t="n">
+        <v>-1.21894769</v>
+      </c>
+      <c r="H3" s="1" t="n">
+        <v>0.536311389</v>
+      </c>
+      <c r="I3" s="1" t="n">
+        <v>1.905036884</v>
+      </c>
+      <c r="J3" s="1" t="n">
+        <v>-89.934</v>
+      </c>
+      <c r="K3" s="1" t="n">
+        <v>-13.33</v>
+      </c>
+      <c r="L3" s="1" t="n">
+        <v>5.64</v>
+      </c>
+      <c r="ALL3" s="0"/>
+      <c r="ALM3" s="0"/>
+      <c r="ALN3" s="0"/>
+      <c r="ALO3" s="0"/>
+      <c r="ALP3" s="0"/>
+      <c r="ALQ3" s="0"/>
+      <c r="ALR3" s="0"/>
+      <c r="ALS3" s="0"/>
+      <c r="ALT3" s="0"/>
+      <c r="ALU3" s="0"/>
+      <c r="ALV3" s="0"/>
+      <c r="ALW3" s="0"/>
+      <c r="ALX3" s="0"/>
+      <c r="ALY3" s="0"/>
+      <c r="ALZ3" s="0"/>
+      <c r="AMA3" s="0"/>
+      <c r="AMB3" s="0"/>
+      <c r="AMC3" s="0"/>
+      <c r="AMD3" s="0"/>
+      <c r="AME3" s="0"/>
+      <c r="AMF3" s="0"/>
+      <c r="AMG3" s="0"/>
+      <c r="AMH3" s="0"/>
+      <c r="AMI3" s="0"/>
+      <c r="AMJ3" s="0"/>
+    </row>
+    <row r="4" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>0.48408665</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>0.27432885</v>
+      </c>
+      <c r="G4" s="1" t="n">
+        <v>-1.13668387</v>
+      </c>
+      <c r="H4" s="1" t="n">
+        <v>0.591529624</v>
+      </c>
+      <c r="I4" s="1" t="n">
+        <v>1.875389224</v>
+      </c>
+      <c r="L4" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="ALL4" s="0"/>
+      <c r="ALM4" s="0"/>
+      <c r="ALN4" s="0"/>
+      <c r="ALO4" s="0"/>
+      <c r="ALP4" s="0"/>
+      <c r="ALQ4" s="0"/>
+      <c r="ALR4" s="0"/>
+      <c r="ALS4" s="0"/>
+      <c r="ALT4" s="0"/>
+      <c r="ALU4" s="0"/>
+      <c r="ALV4" s="0"/>
+      <c r="ALW4" s="0"/>
+      <c r="ALX4" s="0"/>
+      <c r="ALY4" s="0"/>
+      <c r="ALZ4" s="0"/>
+      <c r="AMA4" s="0"/>
+      <c r="AMB4" s="0"/>
+      <c r="AMC4" s="0"/>
+      <c r="AMD4" s="0"/>
+      <c r="AME4" s="0"/>
+      <c r="AMF4" s="0"/>
+      <c r="AMG4" s="0"/>
+      <c r="AMH4" s="0"/>
+      <c r="AMI4" s="0"/>
+      <c r="AMJ4" s="0"/>
+    </row>
+    <row r="5" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>1.278977223</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>0.327921653</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>-0.858380191</v>
+      </c>
+      <c r="H5" s="1" t="n">
+        <v>1.446107084</v>
+      </c>
+      <c r="I5" s="1" t="n">
+        <v>1.736025708</v>
+      </c>
+      <c r="J5" s="1" t="n">
+        <v>-78.101</v>
+      </c>
+      <c r="K5" s="1" t="n">
+        <v>-11.582</v>
+      </c>
+      <c r="L5" s="1" t="n">
+        <v>8.74</v>
+      </c>
+      <c r="ALL5" s="0"/>
+      <c r="ALM5" s="0"/>
+      <c r="ALN5" s="0"/>
+      <c r="ALO5" s="0"/>
+      <c r="ALP5" s="0"/>
+      <c r="ALQ5" s="0"/>
+      <c r="ALR5" s="0"/>
+      <c r="ALS5" s="0"/>
+      <c r="ALT5" s="0"/>
+      <c r="ALU5" s="0"/>
+      <c r="ALV5" s="0"/>
+      <c r="ALW5" s="0"/>
+      <c r="ALX5" s="0"/>
+      <c r="ALY5" s="0"/>
+      <c r="ALZ5" s="0"/>
+      <c r="AMA5" s="0"/>
+      <c r="AMB5" s="0"/>
+      <c r="AMC5" s="0"/>
+      <c r="AMD5" s="0"/>
+      <c r="AME5" s="0"/>
+      <c r="AMF5" s="0"/>
+      <c r="AMG5" s="0"/>
+      <c r="AMH5" s="0"/>
+      <c r="AMI5" s="0"/>
+      <c r="AMJ5" s="0"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>1.2092</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>-95.26</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <v>-14.233</v>
+      </c>
+      <c r="L6" s="0" t="n">
+        <v>2.24</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>0.185059359</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>0.132893103</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>-1.12178083</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>0.566001164</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>1.3179</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>-89.353</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <v>-12.731</v>
+      </c>
+      <c r="L7" s="0" t="n">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>-94.197</v>
+      </c>
+      <c r="K8" s="0" t="n">
+        <v>-13.792</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>0.18544433</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>0.210295175</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>-0.778613816</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>0.764609235</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>1.822968034</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>-109.383</v>
+      </c>
+      <c r="K9" s="0" t="n">
+        <v>-15.682</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>-0.028675877</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>0.065905561</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>-1.194941614</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>0.412953444</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>1.683677649</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <v>-85.262</v>
+      </c>
+      <c r="K10" s="0" t="n">
+        <v>-12.252</v>
+      </c>
+    </row>
+    <row r="11" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="1" t="n">
+        <v>4.330232872</v>
+      </c>
+      <c r="F11" s="1" t="n">
+        <v>3.549444341</v>
+      </c>
+      <c r="G11" s="1" t="n">
+        <v>1.993341772</v>
+      </c>
+      <c r="H11" s="1" t="n">
+        <v>26.67682151</v>
+      </c>
+      <c r="I11" s="1" t="n">
+        <v>5.625607653</v>
+      </c>
+      <c r="J11" s="1" t="n">
+        <v>-79.175</v>
+      </c>
+      <c r="K11" s="1" t="n">
+        <v>-11.536</v>
+      </c>
+      <c r="L11" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="ALL11" s="0"/>
+      <c r="ALM11" s="0"/>
+      <c r="ALN11" s="0"/>
+      <c r="ALO11" s="0"/>
+      <c r="ALP11" s="0"/>
+      <c r="ALQ11" s="0"/>
+      <c r="ALR11" s="0"/>
+      <c r="ALS11" s="0"/>
+      <c r="ALT11" s="0"/>
+      <c r="ALU11" s="0"/>
+      <c r="ALV11" s="0"/>
+      <c r="ALW11" s="0"/>
+      <c r="ALX11" s="0"/>
+      <c r="ALY11" s="0"/>
+      <c r="ALZ11" s="0"/>
+      <c r="AMA11" s="0"/>
+      <c r="AMB11" s="0"/>
+      <c r="AMC11" s="0"/>
+      <c r="AMD11" s="0"/>
+      <c r="AME11" s="0"/>
+      <c r="AMF11" s="0"/>
+      <c r="AMG11" s="0"/>
+      <c r="AMH11" s="0"/>
+      <c r="AMI11" s="0"/>
+      <c r="AMJ11" s="0"/>
+    </row>
+    <row r="12" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" s="1" t="n">
+        <v>5.670058776</v>
+      </c>
+      <c r="F12" s="1" t="n">
+        <v>3.957421357</v>
+      </c>
+      <c r="G12" s="1" t="n">
+        <v>2.429970389</v>
+      </c>
+      <c r="H12" s="1" t="n">
+        <v>28.61340414</v>
+      </c>
+      <c r="I12" s="1" t="n">
+        <v>5.501723609</v>
+      </c>
+      <c r="J12" s="1" t="n">
+        <v>-81.472</v>
+      </c>
+      <c r="K12" s="1" t="n">
+        <v>-12.284</v>
+      </c>
+      <c r="L12" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="ALL12" s="0"/>
+      <c r="ALM12" s="0"/>
+      <c r="ALN12" s="0"/>
+      <c r="ALO12" s="0"/>
+      <c r="ALP12" s="0"/>
+      <c r="ALQ12" s="0"/>
+      <c r="ALR12" s="0"/>
+      <c r="ALS12" s="0"/>
+      <c r="ALT12" s="0"/>
+      <c r="ALU12" s="0"/>
+      <c r="ALV12" s="0"/>
+      <c r="ALW12" s="0"/>
+      <c r="ALX12" s="0"/>
+      <c r="ALY12" s="0"/>
+      <c r="ALZ12" s="0"/>
+      <c r="AMA12" s="0"/>
+      <c r="AMB12" s="0"/>
+      <c r="AMC12" s="0"/>
+      <c r="AMD12" s="0"/>
+      <c r="AME12" s="0"/>
+      <c r="AMF12" s="0"/>
+      <c r="AMG12" s="0"/>
+      <c r="AMH12" s="0"/>
+      <c r="AMI12" s="0"/>
+      <c r="AMJ12" s="0"/>
+    </row>
+    <row r="13" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I13" s="1" t="n">
+        <v>4.065669151</v>
+      </c>
+      <c r="J13" s="1" t="n">
+        <v>-50.801</v>
+      </c>
+      <c r="K13" s="1" t="n">
+        <v>-8.426</v>
+      </c>
+      <c r="L13" s="1" t="n">
+        <v>5.2</v>
+      </c>
+      <c r="ALL13" s="0"/>
+      <c r="ALM13" s="0"/>
+      <c r="ALN13" s="0"/>
+      <c r="ALO13" s="0"/>
+      <c r="ALP13" s="0"/>
+      <c r="ALQ13" s="0"/>
+      <c r="ALR13" s="0"/>
+      <c r="ALS13" s="0"/>
+      <c r="ALT13" s="0"/>
+      <c r="ALU13" s="0"/>
+      <c r="ALV13" s="0"/>
+      <c r="ALW13" s="0"/>
+      <c r="ALX13" s="0"/>
+      <c r="ALY13" s="0"/>
+      <c r="ALZ13" s="0"/>
+      <c r="AMA13" s="0"/>
+      <c r="AMB13" s="0"/>
+      <c r="AMC13" s="0"/>
+      <c r="AMD13" s="0"/>
+      <c r="AME13" s="0"/>
+      <c r="AMF13" s="0"/>
+      <c r="AMG13" s="0"/>
+      <c r="AMH13" s="0"/>
+      <c r="AMI13" s="0"/>
+      <c r="AMJ13" s="0"/>
+    </row>
+    <row r="14" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" s="1" t="n">
+        <v>1.878128524</v>
+      </c>
+      <c r="F14" s="1" t="n">
+        <v>0.753155928</v>
+      </c>
+      <c r="G14" s="1" t="n">
+        <v>0.240985995</v>
+      </c>
+      <c r="H14" s="1" t="n">
+        <v>3.508331025</v>
+      </c>
+      <c r="I14" s="1" t="n">
+        <v>3.04384406</v>
+      </c>
+      <c r="L14" s="1" t="n">
+        <v>3.76</v>
+      </c>
+      <c r="ALL14" s="0"/>
+      <c r="ALM14" s="0"/>
+      <c r="ALN14" s="0"/>
+      <c r="ALO14" s="0"/>
+      <c r="ALP14" s="0"/>
+      <c r="ALQ14" s="0"/>
+      <c r="ALR14" s="0"/>
+      <c r="ALS14" s="0"/>
+      <c r="ALT14" s="0"/>
+      <c r="ALU14" s="0"/>
+      <c r="ALV14" s="0"/>
+      <c r="ALW14" s="0"/>
+      <c r="ALX14" s="0"/>
+      <c r="ALY14" s="0"/>
+      <c r="ALZ14" s="0"/>
+      <c r="AMA14" s="0"/>
+      <c r="AMB14" s="0"/>
+      <c r="AMC14" s="0"/>
+      <c r="AMD14" s="0"/>
+      <c r="AME14" s="0"/>
+      <c r="AMF14" s="0"/>
+      <c r="AMG14" s="0"/>
+      <c r="AMH14" s="0"/>
+      <c r="AMI14" s="0"/>
+      <c r="AMJ14" s="0"/>
+    </row>
+    <row r="15" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I15" s="1" t="n">
+        <v>2.949201663</v>
+      </c>
+      <c r="J15" s="1" t="n">
+        <v>-89.646</v>
+      </c>
+      <c r="K15" s="1" t="n">
+        <v>-13.065</v>
+      </c>
+      <c r="L15" s="1" t="n">
+        <v>5.01</v>
+      </c>
+      <c r="ALL15" s="0"/>
+      <c r="ALM15" s="0"/>
+      <c r="ALN15" s="0"/>
+      <c r="ALO15" s="0"/>
+      <c r="ALP15" s="0"/>
+      <c r="ALQ15" s="0"/>
+      <c r="ALR15" s="0"/>
+      <c r="ALS15" s="0"/>
+      <c r="ALT15" s="0"/>
+      <c r="ALU15" s="0"/>
+      <c r="ALV15" s="0"/>
+      <c r="ALW15" s="0"/>
+      <c r="ALX15" s="0"/>
+      <c r="ALY15" s="0"/>
+      <c r="ALZ15" s="0"/>
+      <c r="AMA15" s="0"/>
+      <c r="AMB15" s="0"/>
+      <c r="AMC15" s="0"/>
+      <c r="AMD15" s="0"/>
+      <c r="AME15" s="0"/>
+      <c r="AMF15" s="0"/>
+      <c r="AMG15" s="0"/>
+      <c r="AMH15" s="0"/>
+      <c r="AMI15" s="0"/>
+      <c r="AMJ15" s="0"/>
+    </row>
+    <row r="16" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J16" s="1" t="n">
+        <v>-65.565</v>
+      </c>
+      <c r="K16" s="1" t="n">
+        <v>-9.298</v>
+      </c>
+      <c r="ALL16" s="0"/>
+      <c r="ALM16" s="0"/>
+      <c r="ALN16" s="0"/>
+      <c r="ALO16" s="0"/>
+      <c r="ALP16" s="0"/>
+      <c r="ALQ16" s="0"/>
+      <c r="ALR16" s="0"/>
+      <c r="ALS16" s="0"/>
+      <c r="ALT16" s="0"/>
+      <c r="ALU16" s="0"/>
+      <c r="ALV16" s="0"/>
+      <c r="ALW16" s="0"/>
+      <c r="ALX16" s="0"/>
+      <c r="ALY16" s="0"/>
+      <c r="ALZ16" s="0"/>
+      <c r="AMA16" s="0"/>
+      <c r="AMB16" s="0"/>
+      <c r="AMC16" s="0"/>
+      <c r="AMD16" s="0"/>
+      <c r="AME16" s="0"/>
+      <c r="AMF16" s="0"/>
+      <c r="AMG16" s="0"/>
+      <c r="AMH16" s="0"/>
+      <c r="AMI16" s="0"/>
+      <c r="AMJ16" s="0"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>6.780331804</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>4.262023065</v>
+      </c>
+      <c r="G17" s="0" t="n">
+        <v>2.591937815</v>
+      </c>
+      <c r="H17" s="0" t="n">
+        <v>29.03969809</v>
+      </c>
+      <c r="I17" s="0" t="n">
+        <v>6.380104084</v>
+      </c>
+      <c r="J17" s="0" t="n">
+        <v>-90.225</v>
+      </c>
+      <c r="K17" s="0" t="n">
+        <v>-13.668</v>
+      </c>
+      <c r="L17" s="0" t="n">
+        <v>3.53</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>3.132389271</v>
+      </c>
+      <c r="F18" s="0" t="n">
+        <v>0.933349867</v>
+      </c>
+      <c r="G18" s="0" t="n">
+        <v>0.260326343</v>
+      </c>
+      <c r="H18" s="0" t="n">
+        <v>4.436051514</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>1.150758114</v>
+      </c>
+      <c r="F19" s="0" t="n">
+        <v>1.137487804</v>
+      </c>
+      <c r="G19" s="0" t="n">
+        <v>2.130392871</v>
+      </c>
+      <c r="H19" s="0" t="n">
+        <v>4.337064961</v>
+      </c>
+      <c r="I19" s="0" t="n">
+        <v>2.1995</v>
+      </c>
+      <c r="J19" s="0" t="n">
+        <v>-75.524</v>
+      </c>
+      <c r="K19" s="0" t="n">
+        <v>-11.193</v>
+      </c>
+      <c r="L19" s="0" t="n">
+        <v>2.83</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="G24" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="H24" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="I24" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="J24" s="0" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <f aca="false">AVERAGE(I17:I19)</f>
+        <v>4.289802042</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <f aca="false">STDEV(I17:I19)</f>
+        <v>2.95613349725257</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
added table for wrr submission to stdev excel
</commit_message>
<xml_diff>
--- a/data/newrnet-chemistry/RI23_endmember_STDEV.xlsx
+++ b/data/newrnet-chemistry/RI23_endmember_STDEV.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="All data" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="169">
   <si>
     <t xml:space="preserve">Sample ID</t>
   </si>
@@ -357,6 +357,12 @@
     <t xml:space="preserve">Groundwater/baseflow</t>
   </si>
   <si>
+    <t xml:space="preserve">Subwatershed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Endmember type</t>
+  </si>
+  <si>
     <t xml:space="preserve">Si (mg/L)</t>
   </si>
   <si>
@@ -378,181 +384,31 @@
     <t xml:space="preserve">Soil water – Dry transect</t>
   </si>
   <si>
-    <t xml:space="preserve">0.505 ± 0.089</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.335 ± 0.061</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.12 ± 0.10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.568 ± 0.028</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.90 ± 0.02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-91.29 ± 1.89</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-13.28 ± 0.05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5.86 ± 1.04</t>
+    <t xml:space="preserve">0.505 ± 0.089 (3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.335 ± 0.061 (3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.12 ± 0.10 (3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.568 ± 0.028 (3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.90 ± 0.02 (3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-91.29 ± 1.89 (2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-13.28 ± 0.05 (2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.86 ± 1.04 (3)</t>
   </si>
   <si>
     <t xml:space="preserve">Soil water - Wet transect</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.279 ± NA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.328 ± NA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.858 ± NA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.446 ± NA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.736 ± NA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-78.10 ± NA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-11.58 ± NA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8.74 ± NA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.114 ± 0.123</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.137 ± 0.059</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.03 ± 0.17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.58 ± 0.14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.76 ± 0.22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-94.78 ± 8.57</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-13.14 ± 1.24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.46 ± 1.03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5.00 ± 0.95</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.75 ± 0.29</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.21 ± 0.31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27.65 ± 1.37</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5.56 ± 0.09</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-80.32 ± 1.15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-12.41 ± 0.53</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5.73 ± 0.51</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.88 ± NA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.753 ± NA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.241 ± NA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.51 ± NA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.04 ± NA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-77.61 ± 17.01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-11.18 ± 2.03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4.39 ± 0.89</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.69 ± 2.83</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.11 ± 1.68</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.66 ± 1.26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12.6 ± 14.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4.29 ± 2.19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-81.88 ± 7.61</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-12.64 ± 1.26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.13 ± 0.36</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Subwatershed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Endmember type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.505 ± 0.089 (3)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.335 ± 0.061 (3)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.12 ± 0.10 (3)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.568 ± 0.028 (3)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.90 ± 0.02 (3)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-91.29 ± 1.89 (2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-13.28 ± 0.05 (2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5.86 ± 1.04 (3)</t>
   </si>
   <si>
     <t xml:space="preserve">1.279 ± NA (1)</t>
@@ -793,10 +649,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AK34"/>
+  <dimension ref="A1:AK36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2293,98 +2149,108 @@
         <v>2.83</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
-        <v>79</v>
-      </c>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="AF21" s="2"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="AF22" s="2"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="B25" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="C25" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="D25" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="E25" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="F25" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="G25" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="H25" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="I25" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="J25" s="0" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="F27" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="G27" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="H27" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="I27" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="J27" s="0" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
         <v>107</v>
       </c>
-      <c r="B26" s="0" t="n">
+      <c r="B28" s="0" t="n">
         <f aca="false">AVERAGE(U18:U20)</f>
         <v>4.289802042</v>
       </c>
-      <c r="C26" s="0" t="n">
+      <c r="C28" s="0" t="n">
         <f aca="false">STDEV(U18:U20)</f>
         <v>2.95613349725257</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
-        <v>109</v>
-      </c>
-    </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>38</v>
+        <v>109</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>108</v>
+        <v>38</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
         <v>110</v>
       </c>
     </row>
@@ -2404,10 +2270,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2416,27 +2282,27 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.48"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>1</v>
+        <v>111</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>4</v>
+        <v>112</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>28</v>
@@ -2445,425 +2311,209 @@
         <v>29</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4"/>
       <c r="B3" s="4" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4"/>
       <c r="B4" s="4" t="s">
         <v>107</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+    </row>
+    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="E5" s="4" t="s">
+      <c r="B6" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="D6" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="E6" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="F6" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="G6" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="H6" s="4" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="C6" s="4" t="s">
+      <c r="I6" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="J6" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4"/>
       <c r="B7" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="E7" s="4" t="s">
+      <c r="C8" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="D8" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="E8" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="F8" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="I7" s="4" t="s">
+      <c r="G8" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="J7" s="4" t="s">
+      <c r="H8" s="4" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="s">
+      <c r="I8" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="J8" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="J12" s="4" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-    </row>
-    <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="I15" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="J15" s="4" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>205</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="I16" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="J16" s="4" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>210</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>211</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="I17" s="4" t="s">
-        <v>215</v>
-      </c>
-      <c r="J17" s="4" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="4" t="s">
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="4" t="s">
         <v>110</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changed to no3n figs 5 and 6
</commit_message>
<xml_diff>
--- a/data/newrnet-chemistry/RI23_endmember_STDEV.xlsx
+++ b/data/newrnet-chemistry/RI23_endmember_STDEV.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="All data" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="SI Table" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="SI Table w DOC" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Just tracers" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="221">
   <si>
     <t xml:space="preserve">Sample ID</t>
   </si>
@@ -318,7 +319,103 @@
     <t xml:space="preserve">RI23-1061</t>
   </si>
   <si>
-    <t xml:space="preserve">Table 2. Mean concentration values of potential hydrologic ﬂowpath tracers in each end-member. Units for Cl_x0001_..</t>
+    <t xml:space="preserve">RI23-1032</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02/17/2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11:30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Baseflow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stream</t>
+  </si>
+  <si>
+    <t xml:space="preserve">need to verify type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the average of two measurements std only 0.04 though</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RI23-5006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Groundwater</t>
+  </si>
+  <si>
+    <t xml:space="preserve">well - High Pond. TOC log says collected 3/19/2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">High_Pond_031023 is it march 1st or 10th</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grab - MED is it gw though?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RI23-5018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03/10/2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">need to verify bear pond see ICP log</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bear_Pond_031023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RI23-1034</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03/22/2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13:15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pre-event baseflow - labled GW for now</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RI23-1001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02/9/2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13:40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RI23-5008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">well</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mark_well_031623</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RI23-1035</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pre-event</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RI23-1085</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03/31/2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Table 2. Mean concentration values of potential hydrologic ﬂowpath tracers in each end-member. Units for Cl..</t>
   </si>
   <si>
     <t xml:space="preserve">End-member</t>
@@ -357,7 +454,7 @@
     <t xml:space="preserve">Groundwater/baseflow</t>
   </si>
   <si>
-    <t xml:space="preserve">Subwatershed</t>
+    <t xml:space="preserve">Subcatchment</t>
   </si>
   <si>
     <t xml:space="preserve">Endmember type</t>
@@ -378,12 +475,137 @@
     <t xml:space="preserve">Cl (mg/L)</t>
   </si>
   <si>
-    <t xml:space="preserve">TOC (mg/L)</t>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="DejaVu Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">δ</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">D</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">δ18O</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOC (mg/L)</t>
   </si>
   <si>
     <t xml:space="preserve">Soil water – Dry transect</t>
   </si>
   <si>
+    <t xml:space="preserve">5.00 ± 0.95 (2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.75 ± 0.29 (2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.21 ± 0.31 (2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27.65 ± 1.37 (2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.56 ± 0.09 (2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-80.32 ± 1.15 (2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-12.41 ± 0.53 (2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.73 ± 0.51 (2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Soil water - Wet transect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.88 ± NA (1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.753 ± NA (1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.241 ± NA (1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.51 ± NA (1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.04 ± NA (1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-77.61 ± 17.01 (2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-11.18 ± 2.03 (2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.39 ± 0.89 (2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meltwater</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.69 ± 2.83 (3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.11 ± 1.68 (3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.66 ± 1.26 (3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12.60 ± 14.3 (3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.29 ± 2.19 (2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-81.88 ± 7.61 (2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-12.64 ± 1.26 (2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.13 ± 0.36 (2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.73 ± 2.65</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12.4 ± 9.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18.3 ± 3.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">64.9 ± 27.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">41.9 ± 14.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-71.9 ± 4.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-10.7 ± 0.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13.7 ± 10.5</t>
+  </si>
+  <si>
     <t xml:space="preserve">0.505 ± 0.089 (3)</t>
   </si>
   <si>
@@ -408,9 +630,6 @@
     <t xml:space="preserve">5.86 ± 1.04 (3)</t>
   </si>
   <si>
-    <t xml:space="preserve">Soil water - Wet transect</t>
-  </si>
-  <si>
     <t xml:space="preserve">1.279 ± NA (1)</t>
   </si>
   <si>
@@ -459,76 +678,31 @@
     <t xml:space="preserve">1.46 ± 1.03 (2)</t>
   </si>
   <si>
-    <t xml:space="preserve">5.00 ± 0.95 (2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.75 ± 0.29 (2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.21 ± 0.31 (2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27.65 ± 1.37 (2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5.56 ± 0.09 (2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-80.32 ± 1.15 (2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-12.41 ± 0.53 (2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5.73 ± 0.51 (2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.88 ± NA (1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.753 ± NA (1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.241 ± NA (1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.51 ± NA (1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.04 ± NA (1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-77.61 ± 17.01 (2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-11.18 ± 2.03 (2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4.39 ± 0.89 (2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.69 ± 2.83 (3)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.11 ± 1.68 (3)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.66 ± 1.26 (3)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12.60 ± 14.3 (3)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4.29 ± 2.19 (2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-81.88 ± 7.61 (2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-12.64 ± 1.26 (2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.13 ± 0.36 (2)</t>
+    <t xml:space="preserve">1.49 ± 0.575 (4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.541 ± 0.202 (4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.58 ± 0.22 (4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.80 ± 1.84 (4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.39 ± 0.42 (4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-77.5 ± 4.3 (4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-11.7 ± 0.4 (4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.12 ± 1.00 (4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Table 2. Mean concentration values of potential hydrologic ﬂowpath tracers in each end-member type for Hungerford and Wade Brook subcatchments.</t>
   </si>
 </sst>
 </file>
@@ -539,12 +713,11 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -566,7 +739,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="DejaVu Sans"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -611,7 +789,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -628,8 +806,16 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -649,13 +835,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AK36"/>
+  <dimension ref="A1:AK46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="S13" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AG32" activeCellId="0" sqref="AG32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="28.16"/>
   </cols>
@@ -2155,103 +2341,1184 @@
       <c r="AF21" s="2"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="AF22" s="2"/>
+      <c r="A22" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="G22" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="I22" s="0" t="n">
+        <v>-0.001828615</v>
+      </c>
+      <c r="J22" s="0" t="n">
+        <v>-0.002236324</v>
+      </c>
+      <c r="K22" s="0" t="n">
+        <v>-0.00145954</v>
+      </c>
+      <c r="L22" s="0" t="n">
+        <v>-0.004198752</v>
+      </c>
+      <c r="M22" s="0" t="n">
+        <v>0.635231917</v>
+      </c>
+      <c r="N22" s="0" t="n">
+        <v>0.232023301</v>
+      </c>
+      <c r="O22" s="0" t="n">
+        <v>-0.015775932</v>
+      </c>
+      <c r="P22" s="0" t="n">
+        <v>0.386433348</v>
+      </c>
+      <c r="Q22" s="0" t="n">
+        <v>-0.796006763</v>
+      </c>
+      <c r="R22" s="0" t="n">
+        <v>0.010952677</v>
+      </c>
+      <c r="S22" s="0" t="n">
+        <v>2.853683177</v>
+      </c>
+      <c r="U22" s="0" t="n">
+        <v>1.0107</v>
+      </c>
+      <c r="X22" s="0" t="n">
+        <v>1.7933</v>
+      </c>
+      <c r="Y22" s="0" t="n">
+        <v>1.1908</v>
+      </c>
+      <c r="Z22" s="0" t="n">
+        <v>3.6512</v>
+      </c>
+      <c r="AC22" s="0" t="n">
+        <v>-80.657</v>
+      </c>
+      <c r="AD22" s="0" t="n">
+        <v>-12.075</v>
+      </c>
+      <c r="AF22" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG22" s="0" t="n">
+        <v>1.68</v>
+      </c>
+      <c r="AH22" s="0" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="G23" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="H23" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="I23" s="0" t="n">
+        <v>-0.008999159</v>
+      </c>
+      <c r="J23" s="0" t="n">
+        <v>-0.003347686</v>
+      </c>
+      <c r="K23" s="0" t="n">
+        <v>-0.000665278</v>
+      </c>
+      <c r="L23" s="0" t="n">
+        <v>-0.000761201</v>
+      </c>
+      <c r="M23" s="0" t="n">
+        <v>1.883644279</v>
+      </c>
+      <c r="N23" s="0" t="n">
+        <v>0.28598758</v>
+      </c>
+      <c r="O23" s="0" t="n">
+        <v>-0.019510879</v>
+      </c>
+      <c r="P23" s="0" t="n">
+        <v>0.425312813</v>
+      </c>
+      <c r="Q23" s="0" t="n">
+        <v>-0.282933665</v>
+      </c>
+      <c r="R23" s="0" t="n">
+        <v>0.00428736</v>
+      </c>
+      <c r="S23" s="0" t="n">
+        <v>6.847131002</v>
+      </c>
+      <c r="U23" s="0" t="n">
+        <v>1.752880691</v>
+      </c>
+      <c r="X23" s="0" t="n">
+        <v>1.717066079</v>
+      </c>
+      <c r="Z23" s="0" t="n">
+        <v>10.92170103</v>
+      </c>
+      <c r="AA23" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC23" s="0" t="n">
+        <v>-76.119</v>
+      </c>
+      <c r="AD23" s="0" t="n">
+        <v>-11.57</v>
+      </c>
+      <c r="AE23" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="AF23" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG23" s="0" t="n">
+        <v>0.07</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="G24" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="H24" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="I24" s="0" t="n">
+        <v>-0.006055875</v>
+      </c>
+      <c r="J24" s="0" t="n">
+        <v>-0.003026873</v>
+      </c>
+      <c r="K24" s="0" t="n">
+        <v>-0.001228727</v>
+      </c>
+      <c r="L24" s="0" t="n">
+        <v>-0.005499911</v>
+      </c>
+      <c r="M24" s="0" t="n">
+        <v>1.689151505</v>
+      </c>
+      <c r="N24" s="0" t="n">
+        <v>0.181631256</v>
+      </c>
+      <c r="O24" s="0" t="n">
+        <v>-0.01777371</v>
+      </c>
+      <c r="P24" s="0" t="n">
+        <v>0.831397948</v>
+      </c>
+      <c r="Q24" s="0" t="n">
+        <v>-0.548253279</v>
+      </c>
+      <c r="R24" s="0" t="n">
+        <v>0.015540279</v>
+      </c>
+      <c r="S24" s="0" t="n">
+        <v>5.788055452</v>
+      </c>
+      <c r="U24" s="0" t="n">
+        <v>1.752880691</v>
+      </c>
+      <c r="AC24" s="0" t="n">
+        <v>-72.071</v>
+      </c>
+      <c r="AD24" s="0" t="n">
+        <v>-11.116</v>
+      </c>
+      <c r="AE24" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="AF24" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG24" s="0" t="n">
+        <v>0.52</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>98</v>
+        <v>114</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="F25" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="G25" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="I25" s="0" t="n">
+        <v>0.014531273</v>
+      </c>
+      <c r="J25" s="0" t="n">
+        <v>-0.000324202</v>
+      </c>
+      <c r="K25" s="0" t="n">
+        <v>-0.001263254</v>
+      </c>
+      <c r="L25" s="0" t="n">
+        <v>-0.001188526</v>
+      </c>
+      <c r="M25" s="0" t="n">
+        <v>1.74915951</v>
+      </c>
+      <c r="N25" s="0" t="n">
+        <v>0.259249227</v>
+      </c>
+      <c r="O25" s="0" t="n">
+        <v>-0.012961239</v>
+      </c>
+      <c r="P25" s="0" t="n">
+        <v>0.522326467</v>
+      </c>
+      <c r="Q25" s="0" t="n">
+        <v>-0.721376146</v>
+      </c>
+      <c r="R25" s="0" t="n">
+        <v>0.029131806</v>
+      </c>
+      <c r="S25" s="0" t="n">
+        <v>3.704749272</v>
+      </c>
+      <c r="U25" s="0" t="n">
+        <v>1.0499</v>
+      </c>
+      <c r="V25" s="0" t="n">
+        <v>0.4131</v>
+      </c>
+      <c r="X25" s="0" t="n">
+        <v>1.6848</v>
+      </c>
+      <c r="Y25" s="0" t="n">
+        <v>1.1272</v>
+      </c>
+      <c r="Z25" s="0" t="n">
+        <v>4.6922</v>
+      </c>
+      <c r="AC25" s="0" t="n">
+        <v>-81.364</v>
+      </c>
+      <c r="AD25" s="0" t="n">
+        <v>-12.059</v>
+      </c>
+      <c r="AF25" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG25" s="0" t="n">
+        <v>2.23</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
-        <v>79</v>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="I26" s="0" t="n">
+        <f aca="false">AVERAGE(I22:I25)</f>
+        <v>-0.000588094</v>
+      </c>
+      <c r="J26" s="0" t="n">
+        <f aca="false">AVERAGE(J22:J25)</f>
+        <v>-0.00223377125</v>
+      </c>
+      <c r="K26" s="0" t="n">
+        <f aca="false">AVERAGE(K22:K25)</f>
+        <v>-0.00115419975</v>
+      </c>
+      <c r="L26" s="0" t="n">
+        <f aca="false">AVERAGE(L22:L25)</f>
+        <v>-0.0029120975</v>
+      </c>
+      <c r="M26" s="0" t="n">
+        <f aca="false">AVERAGE(M22:M25)</f>
+        <v>1.48929680275</v>
+      </c>
+      <c r="N26" s="0" t="n">
+        <f aca="false">AVERAGE(N22:N25)</f>
+        <v>0.239722841</v>
+      </c>
+      <c r="O26" s="0" t="n">
+        <f aca="false">AVERAGE(O22:O25)</f>
+        <v>-0.01650544</v>
+      </c>
+      <c r="P26" s="0" t="n">
+        <f aca="false">AVERAGE(P22:P25)</f>
+        <v>0.541367644</v>
+      </c>
+      <c r="Q26" s="0" t="n">
+        <f aca="false">AVERAGE(Q22:Q25)</f>
+        <v>-0.58714246325</v>
+      </c>
+      <c r="R26" s="0" t="n">
+        <f aca="false">AVERAGE(R22:R25)</f>
+        <v>0.0149780305</v>
+      </c>
+      <c r="S26" s="0" t="n">
+        <f aca="false">AVERAGE(S22:S25)</f>
+        <v>4.79840472575</v>
+      </c>
+      <c r="T26" s="0" t="e">
+        <f aca="false">AVERAGE(T22:T25)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U26" s="0" t="n">
+        <f aca="false">AVERAGE(U22:U25)</f>
+        <v>1.3915903455</v>
+      </c>
+      <c r="V26" s="0" t="n">
+        <f aca="false">AVERAGE(V22:V25)</f>
+        <v>0.4131</v>
+      </c>
+      <c r="W26" s="0" t="e">
+        <f aca="false">AVERAGE(W22:W25)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="X26" s="0" t="n">
+        <f aca="false">AVERAGE(X22:X25)</f>
+        <v>1.73172202633333</v>
+      </c>
+      <c r="Y26" s="0" t="n">
+        <f aca="false">AVERAGE(Y22:Y25)</f>
+        <v>1.159</v>
+      </c>
+      <c r="Z26" s="0" t="n">
+        <f aca="false">AVERAGE(Z22:Z25)</f>
+        <v>6.42170034333333</v>
+      </c>
+      <c r="AA26" s="0" t="e">
+        <f aca="false">AVERAGE(AA22:AA25)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB26" s="0" t="e">
+        <f aca="false">AVERAGE(AB22:AB25)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC26" s="0" t="n">
+        <f aca="false">AVERAGE(AC22:AC25)</f>
+        <v>-77.55275</v>
+      </c>
+      <c r="AD26" s="0" t="n">
+        <f aca="false">AVERAGE(AD22:AD25)</f>
+        <v>-11.705</v>
+      </c>
+      <c r="AE26" s="0" t="e">
+        <f aca="false">AVERAGE(AE22:AE25)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AF26" s="0" t="e">
+        <f aca="false">AVERAGE(AF22:AF25)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AG26" s="0" t="n">
+        <f aca="false">AVERAGE(AG22:AG25)</f>
+        <v>1.125</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="B27" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="C27" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="D27" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="E27" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="F27" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="G27" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="H27" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="I27" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="J27" s="0" t="s">
-        <v>106</v>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="I27" s="0" t="n">
+        <f aca="false">STDEV(I22:I25)</f>
+        <v>0.0105004252982171</v>
+      </c>
+      <c r="J27" s="0" t="n">
+        <f aca="false">STDEV(J22:J25)</f>
+        <v>0.00135600856600032</v>
+      </c>
+      <c r="K27" s="0" t="n">
+        <f aca="false">STDEV(K22:K25)</f>
+        <v>0.000341430464530603</v>
+      </c>
+      <c r="L27" s="0" t="n">
+        <f aca="false">STDEV(L22:L25)</f>
+        <v>0.00230574015466307</v>
+      </c>
+      <c r="M27" s="0" t="n">
+        <f aca="false">STDEV(M22:M25)</f>
+        <v>0.575154266183326</v>
+      </c>
+      <c r="N27" s="0" t="n">
+        <f aca="false">STDEV(N22:N25)</f>
+        <v>0.0445556617763405</v>
+      </c>
+      <c r="O27" s="0" t="n">
+        <f aca="false">STDEV(O22:O25)</f>
+        <v>0.0028127516199199</v>
+      </c>
+      <c r="P27" s="0" t="n">
+        <f aca="false">STDEV(P22:P25)</f>
+        <v>0.201621347691931</v>
+      </c>
+      <c r="Q27" s="0" t="n">
+        <f aca="false">STDEV(Q22:Q25)</f>
+        <v>0.227814499742682</v>
+      </c>
+      <c r="R27" s="0" t="n">
+        <f aca="false">STDEV(R22:R25)</f>
+        <v>0.0105061789885712</v>
+      </c>
+      <c r="S27" s="0" t="n">
+        <f aca="false">STDEV(S22:S25)</f>
+        <v>1.83981086606333</v>
+      </c>
+      <c r="T27" s="0" t="e">
+        <f aca="false">STDEV(T22:T25)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U27" s="0" t="n">
+        <f aca="false">STDEV(U22:U25)</f>
+        <v>0.417488991873254</v>
+      </c>
+      <c r="V27" s="0" t="e">
+        <f aca="false">STDEV(V22:V25)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W27" s="0" t="e">
+        <f aca="false">STDEV(W22:W25)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="X27" s="0" t="n">
+        <f aca="false">STDEV(X22:X25)</f>
+        <v>0.0557149898517272</v>
+      </c>
+      <c r="Y27" s="0" t="n">
+        <f aca="false">STDEV(Y22:Y25)</f>
+        <v>0.0449719912834645</v>
+      </c>
+      <c r="Z27" s="0" t="n">
+        <f aca="false">STDEV(Z22:Z25)</f>
+        <v>3.93172034674395</v>
+      </c>
+      <c r="AA27" s="0" t="e">
+        <f aca="false">STDEV(AA22:AA25)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB27" s="0" t="e">
+        <f aca="false">STDEV(AB22:AB25)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC27" s="0" t="n">
+        <f aca="false">STDEV(AC22:AC25)</f>
+        <v>4.33078964123942</v>
+      </c>
+      <c r="AD27" s="0" t="n">
+        <f aca="false">STDEV(AD22:AD25)</f>
+        <v>0.457297131706144</v>
+      </c>
+      <c r="AE27" s="0" t="e">
+        <f aca="false">STDEV(AE22:AE25)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AF27" s="0" t="e">
+        <f aca="false">STDEV(AF22:AF25)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AG27" s="0" t="n">
+        <f aca="false">STDEV(AG22:AG25)</f>
+        <v>1.00134908997812</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="B28" s="0" t="n">
+        <v>118</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="G28" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="I28" s="0" t="n">
+        <v>0.07070274</v>
+      </c>
+      <c r="J28" s="0" t="n">
+        <v>0.065629733</v>
+      </c>
+      <c r="K28" s="0" t="n">
+        <v>0.000484385</v>
+      </c>
+      <c r="L28" s="0" t="n">
+        <v>0.03255743</v>
+      </c>
+      <c r="M28" s="0" t="n">
+        <v>3.058230455</v>
+      </c>
+      <c r="N28" s="0" t="n">
+        <v>2.587608353</v>
+      </c>
+      <c r="O28" s="0" t="n">
+        <v>0.034568565</v>
+      </c>
+      <c r="P28" s="0" t="n">
+        <v>8.758447425</v>
+      </c>
+      <c r="Q28" s="0" t="n">
+        <v>19.9942659</v>
+      </c>
+      <c r="R28" s="0" t="n">
+        <v>-0.083201787</v>
+      </c>
+      <c r="S28" s="0" t="n">
+        <v>57.31774663</v>
+      </c>
+      <c r="U28" s="0" t="n">
+        <v>36.24354745</v>
+      </c>
+      <c r="X28" s="0" t="n">
+        <v>13.79784939</v>
+      </c>
+      <c r="Z28" s="0" t="n">
+        <v>50.59468528</v>
+      </c>
+      <c r="AA28" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC28" s="0" t="n">
+        <v>-66.095</v>
+      </c>
+      <c r="AD28" s="0" t="n">
+        <v>-9.827</v>
+      </c>
+      <c r="AF28" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG28" s="0" t="n">
+        <v>26.08</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E29" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="F29" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="G29" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="H29" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="I29" s="0" t="n">
+        <v>-0.017935714</v>
+      </c>
+      <c r="J29" s="0" t="n">
+        <v>0.045289908</v>
+      </c>
+      <c r="K29" s="0" t="n">
+        <v>0.035849962</v>
+      </c>
+      <c r="L29" s="0" t="n">
+        <v>0.029241819</v>
+      </c>
+      <c r="M29" s="0" t="n">
+        <v>7.648743775</v>
+      </c>
+      <c r="N29" s="0" t="n">
+        <v>4.438201407</v>
+      </c>
+      <c r="O29" s="0" t="n">
+        <v>0.354392502</v>
+      </c>
+      <c r="P29" s="0" t="n">
+        <v>26.4284451</v>
+      </c>
+      <c r="Q29" s="0" t="n">
+        <v>21.02279844</v>
+      </c>
+      <c r="R29" s="0" t="n">
+        <v>-0.131898869</v>
+      </c>
+      <c r="S29" s="0" t="n">
+        <v>105.9045741</v>
+      </c>
+      <c r="T29" s="0" t="n">
+        <v>0.015458651</v>
+      </c>
+      <c r="U29" s="0" t="n">
+        <v>60.24839626</v>
+      </c>
+      <c r="V29" s="0" t="n">
+        <v>0.857020045</v>
+      </c>
+      <c r="W29" s="0" t="n">
+        <v>1.605056166</v>
+      </c>
+      <c r="X29" s="0" t="n">
+        <v>3.983550327</v>
+      </c>
+      <c r="Y29" s="0" t="n">
+        <v>1.58724521</v>
+      </c>
+      <c r="Z29" s="0" t="n">
+        <v>83.82824622</v>
+      </c>
+      <c r="AA29" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC29" s="0" t="n">
+        <v>-72.633</v>
+      </c>
+      <c r="AD29" s="0" t="n">
+        <v>-10.806</v>
+      </c>
+      <c r="AE29" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="AF29" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG29" s="0" t="n">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="F30" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="G30" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="I30" s="0" t="n">
+        <v>0.080686091</v>
+      </c>
+      <c r="J30" s="0" t="n">
+        <v>0.039445908</v>
+      </c>
+      <c r="K30" s="0" t="n">
+        <v>0.000206012</v>
+      </c>
+      <c r="L30" s="0" t="n">
+        <v>0.002716037</v>
+      </c>
+      <c r="M30" s="0" t="n">
+        <v>2.304313123</v>
+      </c>
+      <c r="N30" s="0" t="n">
+        <v>3.343251836</v>
+      </c>
+      <c r="O30" s="0" t="n">
+        <v>0.054388067</v>
+      </c>
+      <c r="P30" s="0" t="n">
+        <v>8.181779886</v>
+      </c>
+      <c r="Q30" s="0" t="n">
+        <v>18.24564446</v>
+      </c>
+      <c r="R30" s="0" t="n">
+        <v>-0.025073046</v>
+      </c>
+      <c r="S30" s="0" t="n">
+        <v>51.81826641</v>
+      </c>
+      <c r="T30" s="0" t="n">
+        <v>0.1418</v>
+      </c>
+      <c r="U30" s="0" t="n">
+        <v>44.9281</v>
+      </c>
+      <c r="X30" s="0" t="n">
+        <v>25.7819</v>
+      </c>
+      <c r="Z30" s="0" t="n">
+        <v>26.9727</v>
+      </c>
+      <c r="AC30" s="0" t="n">
+        <v>-75.462</v>
+      </c>
+      <c r="AD30" s="0" t="n">
+        <v>-11.153</v>
+      </c>
+      <c r="AF30" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG30" s="0" t="n">
+        <v>7.16</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E31" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="F31" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="G31" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="I31" s="0" t="n">
+        <v>0.060061922</v>
+      </c>
+      <c r="J31" s="0" t="n">
+        <v>0.017483861</v>
+      </c>
+      <c r="K31" s="0" t="n">
+        <v>0.000458481</v>
+      </c>
+      <c r="L31" s="0" t="n">
+        <v>-0.009881379</v>
+      </c>
+      <c r="M31" s="0" t="n">
+        <v>1.922939017</v>
+      </c>
+      <c r="N31" s="0" t="n">
+        <v>1.907550724</v>
+      </c>
+      <c r="O31" s="0" t="n">
+        <v>0.020223105</v>
+      </c>
+      <c r="P31" s="0" t="n">
+        <v>6.349480788</v>
+      </c>
+      <c r="Q31" s="0" t="n">
+        <v>14.15258709</v>
+      </c>
+      <c r="R31" s="0" t="n">
+        <v>-0.061110235</v>
+      </c>
+      <c r="S31" s="0" t="n">
+        <v>44.48903756</v>
+      </c>
+      <c r="T31" s="0" t="n">
+        <v>0.0186</v>
+      </c>
+      <c r="U31" s="0" t="n">
+        <v>26.0618</v>
+      </c>
+      <c r="X31" s="0" t="n">
+        <v>12.1689</v>
+      </c>
+      <c r="Y31" s="0" t="n">
+        <v>2.411</v>
+      </c>
+      <c r="Z31" s="0" t="n">
+        <v>17.2364</v>
+      </c>
+      <c r="AC31" s="0" t="n">
+        <v>-73.371</v>
+      </c>
+      <c r="AD31" s="0" t="n">
+        <v>-11.14</v>
+      </c>
+      <c r="AF31" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG31" s="0" t="n">
+        <v>7.77</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="I32" s="0" t="n">
+        <f aca="false">AVERAGE(I28:I31)</f>
+        <v>0.04837875975</v>
+      </c>
+      <c r="J32" s="0" t="n">
+        <f aca="false">AVERAGE(J28:J31)</f>
+        <v>0.0419623525</v>
+      </c>
+      <c r="K32" s="0" t="n">
+        <f aca="false">AVERAGE(K28:K31)</f>
+        <v>0.00924971</v>
+      </c>
+      <c r="L32" s="0" t="n">
+        <f aca="false">AVERAGE(L28:L31)</f>
+        <v>0.01365847675</v>
+      </c>
+      <c r="M32" s="0" t="n">
+        <f aca="false">AVERAGE(M28:M31)</f>
+        <v>3.7335565925</v>
+      </c>
+      <c r="N32" s="0" t="n">
+        <f aca="false">AVERAGE(N28:N31)</f>
+        <v>3.06915308</v>
+      </c>
+      <c r="O32" s="0" t="n">
+        <f aca="false">AVERAGE(O28:O31)</f>
+        <v>0.11589305975</v>
+      </c>
+      <c r="P32" s="0" t="n">
+        <f aca="false">AVERAGE(P28:P31)</f>
+        <v>12.42953829975</v>
+      </c>
+      <c r="Q32" s="0" t="n">
+        <f aca="false">AVERAGE(Q28:Q31)</f>
+        <v>18.3538239725</v>
+      </c>
+      <c r="R32" s="0" t="n">
+        <f aca="false">AVERAGE(R28:R31)</f>
+        <v>-0.07532098425</v>
+      </c>
+      <c r="S32" s="0" t="n">
+        <f aca="false">AVERAGE(S28:S31)</f>
+        <v>64.882406175</v>
+      </c>
+      <c r="T32" s="0" t="n">
+        <f aca="false">AVERAGE(T28:T31)</f>
+        <v>0.0586195503333333</v>
+      </c>
+      <c r="U32" s="0" t="n">
+        <f aca="false">AVERAGE(U28:U31)</f>
+        <v>41.8704609275</v>
+      </c>
+      <c r="V32" s="0" t="n">
+        <f aca="false">AVERAGE(V28:V31)</f>
+        <v>0.857020045</v>
+      </c>
+      <c r="W32" s="0" t="n">
+        <f aca="false">AVERAGE(W28:W31)</f>
+        <v>1.605056166</v>
+      </c>
+      <c r="X32" s="0" t="n">
+        <f aca="false">AVERAGE(X28:X31)</f>
+        <v>13.93304992925</v>
+      </c>
+      <c r="Y32" s="0" t="n">
+        <f aca="false">AVERAGE(Y28:Y31)</f>
+        <v>1.999122605</v>
+      </c>
+      <c r="Z32" s="0" t="n">
+        <f aca="false">AVERAGE(Z28:Z31)</f>
+        <v>44.658007875</v>
+      </c>
+      <c r="AA32" s="0" t="e">
+        <f aca="false">AVERAGE(AA28:AA31)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB32" s="0" t="e">
+        <f aca="false">AVERAGE(AB28:AB31)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC32" s="0" t="n">
+        <f aca="false">AVERAGE(AC28:AC31)</f>
+        <v>-71.89025</v>
+      </c>
+      <c r="AD32" s="0" t="n">
+        <f aca="false">AVERAGE(AD28:AD31)</f>
+        <v>-10.7315</v>
+      </c>
+      <c r="AE32" s="0" t="e">
+        <f aca="false">AVERAGE(AE28:AE31)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AF32" s="0" t="e">
+        <f aca="false">AVERAGE(AF28:AF31)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AG32" s="0" t="n">
+        <f aca="false">AVERAGE(AG28,AG30:AG31)</f>
+        <v>13.67</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="I33" s="0" t="n">
+        <f aca="false">STDEV(I28:I31)</f>
+        <v>0.0450045533088927</v>
+      </c>
+      <c r="J33" s="0" t="n">
+        <f aca="false">STDEV(J28:J31)</f>
+        <v>0.0198052734086532</v>
+      </c>
+      <c r="K33" s="0" t="n">
+        <f aca="false">STDEV(K28:K31)</f>
+        <v>0.01773394588226</v>
+      </c>
+      <c r="L33" s="0" t="n">
+        <f aca="false">STDEV(L28:L31)</f>
+        <v>0.0206064131282756</v>
+      </c>
+      <c r="M33" s="0" t="n">
+        <f aca="false">STDEV(M28:M31)</f>
+        <v>2.65240953133944</v>
+      </c>
+      <c r="N33" s="0" t="n">
+        <f aca="false">STDEV(N28:N31)</f>
+        <v>1.08483928260803</v>
+      </c>
+      <c r="O33" s="0" t="n">
+        <f aca="false">STDEV(O28:O31)</f>
+        <v>0.159615435526506</v>
+      </c>
+      <c r="P33" s="0" t="n">
+        <f aca="false">STDEV(P28:P31)</f>
+        <v>9.38894475257168</v>
+      </c>
+      <c r="Q33" s="0" t="n">
+        <f aca="false">STDEV(Q28:Q31)</f>
+        <v>3.02636022175538</v>
+      </c>
+      <c r="R33" s="0" t="n">
+        <f aca="false">STDEV(R28:R31)</f>
+        <v>0.0446839448698332</v>
+      </c>
+      <c r="S33" s="0" t="n">
+        <f aca="false">STDEV(S28:S31)</f>
+        <v>27.848420461284</v>
+      </c>
+      <c r="T33" s="0" t="n">
+        <f aca="false">STDEV(T28:T31)</f>
+        <v>0.0720535038943048</v>
+      </c>
+      <c r="U33" s="0" t="n">
+        <f aca="false">STDEV(U28:U31)</f>
+        <v>14.476113421624</v>
+      </c>
+      <c r="V33" s="0" t="e">
+        <f aca="false">STDEV(V28:V31)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W33" s="0" t="e">
+        <f aca="false">STDEV(W28:W31)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="X33" s="0" t="n">
+        <f aca="false">STDEV(X28:X31)</f>
+        <v>8.9910751024367</v>
+      </c>
+      <c r="Y33" s="0" t="n">
+        <f aca="false">STDEV(Y28:Y31)</f>
+        <v>0.5824825980439</v>
+      </c>
+      <c r="Z33" s="0" t="n">
+        <f aca="false">STDEV(Z28:Z31)</f>
+        <v>29.6325631903989</v>
+      </c>
+      <c r="AA33" s="0" t="e">
+        <f aca="false">STDEV(AA28:AA31)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB33" s="0" t="e">
+        <f aca="false">STDEV(AB28:AB31)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC33" s="0" t="n">
+        <f aca="false">STDEV(AC28:AC31)</f>
+        <v>4.04502240414068</v>
+      </c>
+      <c r="AD33" s="0" t="n">
+        <f aca="false">STDEV(AD28:AD31)</f>
+        <v>0.624020565900409</v>
+      </c>
+      <c r="AE33" s="0" t="e">
+        <f aca="false">STDEV(AE28:AE31)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AF33" s="0" t="e">
+        <f aca="false">STDEV(AF28:AF31)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AG33" s="0" t="n">
+        <f aca="false">STDEV(AG28,AG30:AG31)</f>
+        <v>10.7517021908161</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="E37" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="F37" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="G37" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="H37" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="I37" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="J37" s="0" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="B38" s="0" t="n">
         <f aca="false">AVERAGE(U18:U20)</f>
         <v>4.289802042</v>
       </c>
-      <c r="C28" s="0" t="n">
+      <c r="C38" s="0" t="n">
         <f aca="false">STDEV(U18:U20)</f>
         <v>2.95613349725257</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
-        <v>110</v>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -2273,248 +3540,285 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+      <selection pane="topLeft" activeCell="I14" activeCellId="0" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.48"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>111</v>
+        <v>143</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>112</v>
+        <v>144</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>113</v>
+        <v>145</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>114</v>
+        <v>146</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>115</v>
+        <v>147</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>116</v>
+        <v>148</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>28</v>
+        <v>149</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>150</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>29</v>
+        <v>151</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>118</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="H4" s="4" t="s">
+      <c r="B6" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>199</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="I7" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>208</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>209</v>
+      </c>
+      <c r="I8" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="J8" s="0" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="0" t="s">
         <v>142</v>
       </c>
-      <c r="I4" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-    </row>
-    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="4" t="s">
-        <v>110</v>
+      <c r="C9" s="0" t="s">
+        <v>212</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>214</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>215</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>216</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="I9" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="J9" s="0" t="s">
+        <v>219</v>
       </c>
     </row>
   </sheetData>
@@ -2539,7 +3843,7 @@
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="27.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="28.16"/>
@@ -3442,7 +4746,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>98</v>
+        <v>130</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3452,25 +4756,25 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>99</v>
+        <v>131</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>100</v>
+        <v>132</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>101</v>
+        <v>133</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>102</v>
+        <v>134</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>103</v>
+        <v>135</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>104</v>
+        <v>136</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>105</v>
+        <v>137</v>
       </c>
       <c r="H24" s="0" t="s">
         <v>29</v>
@@ -3479,12 +4783,12 @@
         <v>28</v>
       </c>
       <c r="J24" s="0" t="s">
-        <v>106</v>
+        <v>138</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>107</v>
+        <v>139</v>
       </c>
       <c r="B25" s="0" t="n">
         <f aca="false">AVERAGE(I17:I19)</f>
@@ -3497,17 +4801,17 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>108</v>
+        <v>140</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>109</v>
+        <v>141</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>110</v>
+        <v>142</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3517,22 +4821,22 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>107</v>
+        <v>139</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>108</v>
+        <v>140</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>109</v>
+        <v>141</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>110</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -3544,4 +4848,290 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I10"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.48"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="I7" s="0" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>199</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="I8" s="0" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>208</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>209</v>
+      </c>
+      <c r="I9" s="0" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>212</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>214</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>215</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>216</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="I10" s="0" t="s">
+        <v>218</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>